<commit_message>
update program and statictis 1
</commit_message>
<xml_diff>
--- a/TK/thongKe.xlsx
+++ b/TK/thongKe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Class\ky2_2122\XL tín hiệu số\CK\TK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE0FEA2-6AD6-454D-8C54-AD8AFE287194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733623E0-0A14-4568-8907-8F060D51CD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8A0C4B13-D321-42AC-9D1D-8AEB5029EB76}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:M559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -471,14 +471,14 @@
       </c>
       <c r="F2">
         <f>AVERAGE(A2:A46)</f>
-        <v>0</v>
+        <v>7.0222222222222225E-4</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2">
         <f xml:space="preserve"> _xlfn.VAR.S(A2:A46)</f>
-        <v>0</v>
+        <v>1.2771131313131313E-5</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -510,14 +510,14 @@
       </c>
       <c r="F3">
         <f xml:space="preserve"> AVERAGE(A47:A82)</f>
-        <v>5.2888888888888888E-2</v>
+        <v>0.27301944444444454</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3">
         <f xml:space="preserve"> _xlfn.VAR.S(A47:A82)</f>
-        <v>1.1625941015873015E-2</v>
+        <v>0.11651499189682535</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B4">
         <v>1.5900000000000001E-2</v>
@@ -549,14 +549,14 @@
       </c>
       <c r="F4">
         <f xml:space="preserve"> AVERAGE(A83:A154)</f>
-        <v>1.527777777777778E-5</v>
+        <v>9.4444444444444496E-5</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
       <c r="H4">
         <f xml:space="preserve"> _xlfn.VAR.S(A83:A154)</f>
-        <v>2.1576682316118841E-9</v>
+        <v>1.574334898278561E-8</v>
       </c>
       <c r="J4" t="s">
         <v>5</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -588,14 +588,14 @@
       </c>
       <c r="F5">
         <f xml:space="preserve"> AVERAGE(A155:A186)</f>
-        <v>6.3140624999999992E-2</v>
+        <v>0.11874062499999999</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="H5">
         <f xml:space="preserve"> _xlfn.VAR.S(A155:A186)</f>
-        <v>6.2110689415322568E-3</v>
+        <v>1.6484381844758072E-2</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -627,14 +627,14 @@
       </c>
       <c r="F6">
         <f xml:space="preserve"> AVERAGE(A187:A270)</f>
-        <v>4.4047619047619027E-5</v>
+        <v>3.3214285714285713E-4</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
       </c>
       <c r="H6">
         <f xml:space="preserve"> _xlfn.VAR.S(A187:A270)</f>
-        <v>4.9039013195639651E-9</v>
+        <v>5.4822074010327013E-6</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -666,14 +666,14 @@
       </c>
       <c r="F7">
         <f xml:space="preserve"> AVERAGE(A271:A287)</f>
-        <v>8.2894117647058813E-2</v>
+        <v>0.10121176470588236</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
       <c r="H7">
         <f xml:space="preserve"> _xlfn.VAR.S(A271:A287)</f>
-        <v>2.8445480882352964E-3</v>
+        <v>3.7717986029411777E-3</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B8">
         <v>1.5900000000000001E-2</v>
@@ -704,34 +704,34 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <f xml:space="preserve"> AVERAGE(A283:A379)</f>
-        <v>2.0865979381443269E-3</v>
+        <f xml:space="preserve"> AVERAGE(A288:A379)</f>
+        <v>2.3152173913043459E-4</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
       <c r="H8">
-        <f xml:space="preserve"> _xlfn.VAR.S(A283:A379)</f>
-        <v>8.3394089347079019E-5</v>
+        <f xml:space="preserve"> _xlfn.VAR.S(A288:A379)</f>
+        <v>4.2086359292881104E-7</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
       <c r="K8">
-        <f xml:space="preserve"> AVERAGE(B283:B379)</f>
-        <v>0.3294061855670104</v>
+        <f xml:space="preserve"> AVERAGE(B288:B379)</f>
+        <v>0.32953804347826099</v>
       </c>
       <c r="L8" t="s">
         <v>7</v>
       </c>
       <c r="M8">
-        <f xml:space="preserve"> _xlfn.VAR.S(B283:B379)</f>
-        <v>2.1111074753006775E-2</v>
+        <f xml:space="preserve"> _xlfn.VAR.S(B288:B379)</f>
+        <v>2.216769249283318E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -744,14 +744,14 @@
       </c>
       <c r="F9">
         <f xml:space="preserve"> AVERAGE(A380:A416)</f>
-        <v>0.27640540540540548</v>
+        <v>0.24164324324324324</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
       <c r="H9">
         <f xml:space="preserve"> _xlfn.VAR.S(A380:A416)</f>
-        <v>0.11454251108108106</v>
+        <v>8.0058214744744741E-2</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -783,14 +783,14 @@
       </c>
       <c r="F10">
         <f xml:space="preserve"> AVERAGE(A417:A485)</f>
-        <v>1.1884057971014494E-4</v>
+        <v>1.3188405797101452E-4</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
       <c r="H10">
         <f xml:space="preserve"> _xlfn.VAR.S(A417:A485)</f>
-        <v>2.037510656436493E-8</v>
+        <v>1.4220375106564361E-7</v>
       </c>
       <c r="J10" t="s">
         <v>5</v>
@@ -822,14 +822,14 @@
       </c>
       <c r="F11">
         <f xml:space="preserve"> AVERAGE(A486:A515)</f>
-        <v>0.21846333333333334</v>
+        <v>0.14631999999999995</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
       <c r="H11">
         <f xml:space="preserve"> _xlfn.VAR.S(A486:A515)</f>
-        <v>6.0785567919540213E-2</v>
+        <v>2.4303711310344839E-2</v>
       </c>
       <c r="J11" t="s">
         <v>6</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -861,14 +861,14 @@
       </c>
       <c r="F12">
         <f>AVERAGE(A516:A557)</f>
-        <v>8.5714285714285658E-5</v>
+        <v>4.7619047619047627E-5</v>
       </c>
       <c r="G12" t="s">
         <v>7</v>
       </c>
       <c r="H12">
         <f xml:space="preserve"> _xlfn.VAR.S(A516:A557)</f>
-        <v>4.6689895470383289E-9</v>
+        <v>2.5551684088269439E-9</v>
       </c>
       <c r="J12" t="s">
         <v>5</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="B13">
         <v>1.5900000000000001E-2</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -922,24 +922,24 @@
       </c>
       <c r="F15">
         <f xml:space="preserve"> AVERAGE(F2,F4,F6,F8,F10,F12)</f>
-        <v>3.9174636673235905E-4</v>
+        <v>2.5663906142167013E-4</v>
       </c>
       <c r="H15">
         <f xml:space="preserve"> AVERAGE(H2,H4,H6,H8,H10,H12)</f>
-        <v>1.3904365835456934E-5</v>
+        <v>3.1391174292583469E-6</v>
       </c>
       <c r="K15">
         <f xml:space="preserve"> AVERAGE(K2,K4,K6,K8,K10,K12)</f>
-        <v>0.27918430025488955</v>
+        <v>0.27920627657343133</v>
       </c>
       <c r="M15">
         <f xml:space="preserve"> AVERAGE(M2,M4,M6,M8,M10,M12)</f>
-        <v>1.949920561258708E-2</v>
+        <v>1.9675308569224812E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -952,11 +952,11 @@
       </c>
       <c r="F16">
         <f xml:space="preserve"> AVERAGE(F3,F5,F7,F9,F11)</f>
-        <v>0.1387584740549373</v>
+        <v>0.17618701547871402</v>
       </c>
       <c r="H16">
         <f xml:space="preserve"> AVERAGE(H3,H5,H7,H9,H11)</f>
-        <v>3.9201927409252366E-2</v>
+        <v>4.8226619679922839E-2</v>
       </c>
       <c r="K16">
         <f xml:space="preserve"> AVERAGE(K3,K5,K7,K9,K11)</f>
@@ -969,7 +969,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -993,16 +993,16 @@
       </c>
       <c r="G18">
         <f xml:space="preserve"> ((F15 + H15) + (F16 - H16)) / 2</f>
-        <v>4.9981098689126376E-2</v>
+        <v>6.411008698882105E-2</v>
       </c>
       <c r="L18">
         <f xml:space="preserve"> ((K15 + M15) + (K16 - M16)) / 2</f>
-        <v>0.25446720784133769</v>
+        <v>0.25456624747892748</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1011,8 +1011,8 @@
         <v>3</v>
       </c>
       <c r="G19">
-        <f xml:space="preserve"> F15 + H15</f>
-        <v>4.05650732567816E-4</v>
+        <f xml:space="preserve"> F15 - H15</f>
+        <v>2.5349994399241177E-4</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1028,7 +1028,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B21">
         <v>3.1699999999999999E-2</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B22">
         <v>3.1699999999999999E-2</v>
@@ -1047,10 +1047,18 @@
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F22">
+        <f xml:space="preserve"> AVERAGE(A2:A46,A83:A154,A187:A270,A288:A379,A417:A485,A516:A557)</f>
+        <v>2.4430693069307059E-4</v>
+      </c>
+      <c r="H22">
+        <f xml:space="preserve"> _xlfn.VAR.S(A2:A46,A83:A154,A187:A270,A288:A379,A417:A485,A516:A557)</f>
+        <v>2.680786367098244E-6</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B23">
         <v>1.5900000000000001E-2</v>
@@ -1058,10 +1066,14 @@
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G23">
+        <f xml:space="preserve"> F22 - H22</f>
+        <v>2.4162614432597234E-4</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B24">
         <v>3.1699999999999999E-2</v>
@@ -1072,7 +1084,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B25">
         <v>7.9399999999999998E-2</v>
@@ -1082,11 +1094,11 @@
       </c>
       <c r="F25">
         <f xml:space="preserve"> AVERAGE(A2:A46,A83:A154,A187:A270,A288:A379,A417:A485,A516:A557)</f>
-        <v>8.4900990099009944E-5</v>
+        <v>2.4430693069307059E-4</v>
       </c>
       <c r="G25">
         <f xml:space="preserve"> _xlfn.VAR.S(A2:A46,A83:A154,A187:A270,A288:A379,A417:A485,A516:A557)</f>
-        <v>9.269949389479923E-8</v>
+        <v>2.680786367098244E-6</v>
       </c>
       <c r="J25">
         <f xml:space="preserve"> AVERAGE(B2:B46,B83:B154,B187:B270,B288:B379,B417:B485,B516:B557)</f>
@@ -1099,7 +1111,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B26">
         <v>3.1699999999999999E-2</v>
@@ -1109,11 +1121,11 @@
       </c>
       <c r="F26">
         <f xml:space="preserve"> AVERAGE(A47:A82,A155:A186,A271:A287,A380:A416,A486:A515)</f>
-        <v>0.14549078947368421</v>
+        <v>0.18868026315789468</v>
       </c>
       <c r="G26">
         <f xml:space="preserve"> _xlfn.VAR.S(A47:A82,A155:A186,A271:A287,A380:A416,A486:A515)</f>
-        <v>5.2433645609968639E-2</v>
+        <v>5.9182622919135598E-2</v>
       </c>
       <c r="J26">
         <f xml:space="preserve"> AVERAGE(B47:B82,B155:B186,B271:B287,B380:B416,B486:B515)</f>
@@ -1126,7 +1138,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B27">
         <v>7.9399999999999998E-2</v>
@@ -1137,7 +1149,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1147,7 +1159,7 @@
       </c>
       <c r="G28">
         <f xml:space="preserve"> ((F25 + G25) + (F26 - G26)) / 2</f>
-        <v>4.6571068776654241E-2</v>
+        <v>6.4872313977909629E-2</v>
       </c>
       <c r="K28">
         <f xml:space="preserve"> ((J25 + K25) + (J26 - K26)) / 2</f>
@@ -1156,7 +1168,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B29">
         <v>3.1699999999999999E-2</v>
@@ -1167,7 +1179,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B30">
         <v>1.5900000000000001E-2</v>
@@ -1178,7 +1190,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1189,7 +1201,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B32">
         <v>9.5200000000000007E-2</v>
@@ -1200,7 +1212,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B33">
         <v>7.9399999999999998E-2</v>
@@ -1211,7 +1223,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1222,7 +1234,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1233,7 +1245,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1244,7 +1256,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1255,7 +1267,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B38">
         <v>4.7600000000000003E-2</v>
@@ -1266,7 +1278,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B39">
         <v>3.1699999999999999E-2</v>
@@ -1277,7 +1289,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1288,7 +1300,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1299,7 +1311,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1310,7 +1322,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B43">
         <v>1.5900000000000001E-2</v>
@@ -1332,7 +1344,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>0</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="B45">
         <v>4.7600000000000003E-2</v>
@@ -1343,7 +1355,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>0</v>
+        <v>2.4E-2</v>
       </c>
       <c r="B46">
         <v>6.3500000000000001E-2</v>
@@ -1354,7 +1366,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>0</v>
+        <v>7.9600000000000004E-2</v>
       </c>
       <c r="B47">
         <v>1.5900000000000001E-2</v>
@@ -1365,7 +1377,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1.2200000000000001E-2</v>
+        <v>0.18679999999999999</v>
       </c>
       <c r="B48">
         <v>1.5900000000000001E-2</v>
@@ -1376,7 +1388,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>7.9000000000000008E-3</v>
+        <v>0.39889999999999998</v>
       </c>
       <c r="B49">
         <v>1.5900000000000001E-2</v>
@@ -1387,7 +1399,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1.49E-2</v>
+        <v>0.54190000000000005</v>
       </c>
       <c r="B50">
         <v>1.5900000000000001E-2</v>
@@ -1398,7 +1410,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>0.30170000000000002</v>
+        <v>0.62629999999999997</v>
       </c>
       <c r="B51">
         <v>3.1699999999999999E-2</v>
@@ -1409,7 +1421,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>4.6100000000000002E-2</v>
+        <v>0.79149999999999998</v>
       </c>
       <c r="B52">
         <v>3.1699999999999999E-2</v>
@@ -1420,7 +1432,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>1.8700000000000001E-2</v>
+        <v>0.86019999999999996</v>
       </c>
       <c r="B53">
         <v>1.5900000000000001E-2</v>
@@ -1431,7 +1443,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>0.52139999999999997</v>
+        <v>1</v>
       </c>
       <c r="B54">
         <v>3.1699999999999999E-2</v>
@@ -1442,7 +1454,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>0.11409999999999999</v>
+        <v>0.9153</v>
       </c>
       <c r="B55">
         <v>3.1699999999999999E-2</v>
@@ -1453,7 +1465,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>1.01E-2</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="B56">
         <v>3.1699999999999999E-2</v>
@@ -1464,7 +1476,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>0.1855</v>
+        <v>0.81010000000000004</v>
       </c>
       <c r="B57">
         <v>7.9399999999999998E-2</v>
@@ -1475,7 +1487,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>2.5899999999999999E-2</v>
+        <v>0.69679999999999997</v>
       </c>
       <c r="B58">
         <v>3.1699999999999999E-2</v>
@@ -1486,7 +1498,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>0.21479999999999999</v>
+        <v>0.62270000000000003</v>
       </c>
       <c r="B59">
         <v>4.7600000000000003E-2</v>
@@ -1497,7 +1509,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>0.1242</v>
+        <v>0.45850000000000002</v>
       </c>
       <c r="B60">
         <v>3.1699999999999999E-2</v>
@@ -1508,7 +1520,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>1.78E-2</v>
+        <v>0.3458</v>
       </c>
       <c r="B61">
         <v>6.3500000000000001E-2</v>
@@ -1519,7 +1531,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>0.16389999999999999</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="B62">
         <v>4.7600000000000003E-2</v>
@@ -1530,7 +1542,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>6.54E-2</v>
+        <v>0.15060000000000001</v>
       </c>
       <c r="B63">
         <v>3.1699999999999999E-2</v>
@@ -1541,7 +1553,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>7.4999999999999997E-3</v>
+        <v>8.0299999999999996E-2</v>
       </c>
       <c r="B64">
         <v>3.1699999999999999E-2</v>
@@ -1552,7 +1564,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>1.52E-2</v>
+        <v>5.1200000000000002E-2</v>
       </c>
       <c r="B65">
         <v>6.3500000000000001E-2</v>
@@ -1563,7 +1575,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>1.6299999999999999E-2</v>
+        <v>2.7300000000000001E-2</v>
       </c>
       <c r="B66">
         <v>4.7600000000000003E-2</v>
@@ -1574,7 +1586,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>3.3E-3</v>
+        <v>1.49E-2</v>
       </c>
       <c r="B67">
         <v>3.1699999999999999E-2</v>
@@ -1585,7 +1597,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>3.3999999999999998E-3</v>
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="B68">
         <v>0.1111</v>
@@ -1596,7 +1608,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>1.6000000000000001E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="B69">
         <v>4.7600000000000003E-2</v>
@@ -1607,7 +1619,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>2E-3</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="B70">
         <v>4.7600000000000003E-2</v>
@@ -1618,7 +1630,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>1.2999999999999999E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="B71">
         <v>6.3500000000000001E-2</v>
@@ -1629,7 +1641,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>1.6000000000000001E-3</v>
+        <v>5.3E-3</v>
       </c>
       <c r="B72">
         <v>4.7600000000000003E-2</v>
@@ -1640,7 +1652,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>1E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="B73">
         <v>7.9399999999999998E-2</v>
@@ -1651,7 +1663,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>5.0000000000000001E-4</v>
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="B74">
         <v>6.3500000000000001E-2</v>
@@ -1662,7 +1674,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>2.5000000000000001E-3</v>
+        <v>3.8E-3</v>
       </c>
       <c r="B75">
         <v>4.7600000000000003E-2</v>
@@ -1673,7 +1685,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>6.9999999999999999E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="B76">
         <v>4.7600000000000003E-2</v>
@@ -1684,7 +1696,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="B77">
         <v>7.9399999999999998E-2</v>
@@ -1695,7 +1707,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>2.0000000000000001E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="B78">
         <v>3.1699999999999999E-2</v>
@@ -1706,7 +1718,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>2.0000000000000001E-4</v>
+        <v>1.9E-3</v>
       </c>
       <c r="B79">
         <v>4.7600000000000003E-2</v>
@@ -1717,7 +1729,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>5.0000000000000001E-4</v>
+        <v>1.4E-3</v>
       </c>
       <c r="B80">
         <v>3.1699999999999999E-2</v>
@@ -1728,7 +1740,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>5.9999999999999995E-4</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="B81">
         <v>4.7600000000000003E-2</v>
@@ -1750,7 +1762,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>0</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B83">
         <v>7.9399999999999998E-2</v>
@@ -1761,7 +1773,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>0</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="B84">
         <v>0.1111</v>
@@ -1772,7 +1784,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>1E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B85">
         <v>9.5200000000000007E-2</v>
@@ -1783,7 +1795,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>1E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="B86">
         <v>7.9399999999999998E-2</v>
@@ -1794,7 +1806,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>1E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="B87">
         <v>6.3500000000000001E-2</v>
@@ -1838,7 +1850,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B91">
         <v>0.1111</v>
@@ -1849,7 +1861,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B92">
         <v>0.20630000000000001</v>
@@ -1860,7 +1872,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B93">
         <v>0.17460000000000001</v>
@@ -1871,7 +1883,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>0</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B94">
         <v>4.7600000000000003E-2</v>
@@ -1882,7 +1894,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B95">
         <v>9.5200000000000007E-2</v>
@@ -1893,7 +1905,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B96">
         <v>0.1905</v>
@@ -1904,7 +1916,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B97">
         <v>4.7600000000000003E-2</v>
@@ -2025,7 +2037,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B108">
         <v>0.127</v>
@@ -2036,7 +2048,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -2058,7 +2070,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B111">
         <v>0.15870000000000001</v>
@@ -2069,7 +2081,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B112">
         <v>0.1429</v>
@@ -2080,7 +2092,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B113">
         <v>9.5200000000000007E-2</v>
@@ -2190,7 +2202,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B123">
         <v>6.3500000000000001E-2</v>
@@ -2201,7 +2213,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B124">
         <v>0.15870000000000001</v>
@@ -2223,7 +2235,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B126">
         <v>4.7600000000000003E-2</v>
@@ -2234,7 +2246,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B127">
         <v>3.1699999999999999E-2</v>
@@ -2245,7 +2257,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B128">
         <v>4.7600000000000003E-2</v>
@@ -2256,7 +2268,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B129">
         <v>0.1429</v>
@@ -2267,7 +2279,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B130">
         <v>9.5200000000000007E-2</v>
@@ -2278,7 +2290,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B131">
         <v>0.127</v>
@@ -2289,7 +2301,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B132">
         <v>7.9399999999999998E-2</v>
@@ -2300,7 +2312,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B133">
         <v>0.1905</v>
@@ -2344,7 +2356,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B137">
         <v>0.3175</v>
@@ -2355,7 +2367,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B138">
         <v>0.17460000000000001</v>
@@ -2366,7 +2378,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B139">
         <v>0.1429</v>
@@ -2377,7 +2389,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B140">
         <v>7.9399999999999998E-2</v>
@@ -2388,7 +2400,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B141">
         <v>6.3500000000000001E-2</v>
@@ -2399,7 +2411,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B142">
         <v>0.1905</v>
@@ -2410,7 +2422,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B143">
         <v>7.9399999999999998E-2</v>
@@ -2421,7 +2433,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B144">
         <v>3.1699999999999999E-2</v>
@@ -2443,7 +2455,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B146">
         <v>0.17460000000000001</v>
@@ -2454,7 +2466,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B147">
         <v>0.20630000000000001</v>
@@ -2465,7 +2477,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B148">
         <v>0.15870000000000001</v>
@@ -2531,7 +2543,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="B154">
         <v>0.30159999999999998</v>
@@ -2542,7 +2554,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>0</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="B155">
         <v>0.28570000000000001</v>
@@ -2553,7 +2565,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>0</v>
+        <v>1.9E-2</v>
       </c>
       <c r="B156">
         <v>0.15870000000000001</v>
@@ -2564,7 +2576,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>3.3E-3</v>
+        <v>4.7199999999999999E-2</v>
       </c>
       <c r="B157">
         <v>0.1111</v>
@@ -2575,7 +2587,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>1.3899999999999999E-2</v>
+        <v>7.8399999999999997E-2</v>
       </c>
       <c r="B158">
         <v>0.17460000000000001</v>
@@ -2586,7 +2598,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>4.9700000000000001E-2</v>
+        <v>0.10929999999999999</v>
       </c>
       <c r="B159">
         <v>0.15870000000000001</v>
@@ -2597,7 +2609,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>2.46E-2</v>
+        <v>0.18149999999999999</v>
       </c>
       <c r="B160">
         <v>9.5200000000000007E-2</v>
@@ -2608,7 +2620,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>5.7700000000000001E-2</v>
+        <v>0.23719999999999999</v>
       </c>
       <c r="B161">
         <v>0.26979999999999998</v>
@@ -2619,7 +2631,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>0.19650000000000001</v>
+        <v>0.27329999999999999</v>
       </c>
       <c r="B162">
         <v>0.17460000000000001</v>
@@ -2630,7 +2642,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>0.10249999999999999</v>
+        <v>0.29289999999999999</v>
       </c>
       <c r="B163">
         <v>0.17460000000000001</v>
@@ -2641,7 +2653,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>0.13350000000000001</v>
+        <v>0.3014</v>
       </c>
       <c r="B164">
         <v>0.20630000000000001</v>
@@ -2652,7 +2664,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>0.23419999999999999</v>
+        <v>0.32379999999999998</v>
       </c>
       <c r="B165">
         <v>0.20630000000000001</v>
@@ -2663,7 +2675,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>0.1021</v>
+        <v>0.34010000000000001</v>
       </c>
       <c r="B166">
         <v>0.1111</v>
@@ -2674,7 +2686,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>0.1487</v>
+        <v>0.3392</v>
       </c>
       <c r="B167">
         <v>0.17460000000000001</v>
@@ -2685,7 +2697,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>0.29339999999999999</v>
+        <v>0.31409999999999999</v>
       </c>
       <c r="B168">
         <v>0.23810000000000001</v>
@@ -2696,7 +2708,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>0.12529999999999999</v>
+        <v>0.26640000000000003</v>
       </c>
       <c r="B169">
         <v>7.9399999999999998E-2</v>
@@ -2707,7 +2719,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>0.12959999999999999</v>
+        <v>0.21290000000000001</v>
       </c>
       <c r="B170">
         <v>0.20630000000000001</v>
@@ -2718,7 +2730,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>0.161</v>
+        <v>0.17180000000000001</v>
       </c>
       <c r="B171">
         <v>0.17460000000000001</v>
@@ -2729,7 +2741,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>5.2900000000000003E-2</v>
+        <v>0.114</v>
       </c>
       <c r="B172">
         <v>0.1111</v>
@@ -2740,7 +2752,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>6.5600000000000006E-2</v>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="B173">
         <v>0.20630000000000001</v>
@@ -2751,7 +2763,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>8.5199999999999998E-2</v>
+        <v>4.4900000000000002E-2</v>
       </c>
       <c r="B174">
         <v>0.1111</v>
@@ -2762,7 +2774,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>1.34E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="B175">
         <v>0.1905</v>
@@ -2773,7 +2785,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>9.7999999999999997E-3</v>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="B176">
         <v>0.1111</v>
@@ -2784,7 +2796,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>4.1000000000000003E-3</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="B177">
         <v>0.15870000000000001</v>
@@ -2795,7 +2807,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>2.7000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="B178">
         <v>0.127</v>
@@ -2806,7 +2818,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>2E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="B179">
         <v>0.1111</v>
@@ -2817,7 +2829,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>2.0999999999999999E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="B180">
         <v>0.254</v>
@@ -2828,7 +2840,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>3.3E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="B181">
         <v>0.1111</v>
@@ -2839,7 +2851,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>1.1000000000000001E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="B182">
         <v>0.30159999999999998</v>
@@ -2850,7 +2862,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>1E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="B183">
         <v>0.254</v>
@@ -2883,7 +2895,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>1E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B186">
         <v>0.23810000000000001</v>
@@ -2894,7 +2906,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>1E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B187">
         <v>0.254</v>
@@ -2905,7 +2917,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>1E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B188">
         <v>0.3175</v>
@@ -2916,7 +2928,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B189">
         <v>0.26979999999999998</v>
@@ -2927,7 +2939,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B190">
         <v>0.22220000000000001</v>
@@ -2938,7 +2950,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B191">
         <v>0.254</v>
@@ -2960,7 +2972,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B193">
         <v>0.1111</v>
@@ -2971,7 +2983,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B194">
         <v>0.20630000000000001</v>
@@ -2993,7 +3005,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B196">
         <v>0.22220000000000001</v>
@@ -3015,7 +3027,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B198">
         <v>0.22220000000000001</v>
@@ -3026,7 +3038,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B199">
         <v>0.17460000000000001</v>
@@ -3037,7 +3049,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B200">
         <v>0.23810000000000001</v>
@@ -3081,7 +3093,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B204">
         <v>0.127</v>
@@ -3103,7 +3115,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B206">
         <v>0.1905</v>
@@ -3125,7 +3137,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B208">
         <v>0.22220000000000001</v>
@@ -3136,7 +3148,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B209">
         <v>0.28570000000000001</v>
@@ -3180,7 +3192,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B213">
         <v>0.28570000000000001</v>
@@ -3191,7 +3203,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B214">
         <v>0.26979999999999998</v>
@@ -3202,7 +3214,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>2.9999999999999997E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B215">
         <v>0.1905</v>
@@ -3257,7 +3269,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B220">
         <v>0.127</v>
@@ -3323,7 +3335,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B226">
         <v>0.33329999999999999</v>
@@ -3345,7 +3357,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B228">
         <v>0.17460000000000001</v>
@@ -3455,7 +3467,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B238">
         <v>0.28570000000000001</v>
@@ -3466,7 +3478,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B239">
         <v>0.20630000000000001</v>
@@ -3521,7 +3533,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B244">
         <v>0.42859999999999998</v>
@@ -3532,7 +3544,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B245">
         <v>0.3175</v>
@@ -3565,7 +3577,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B248">
         <v>0.34920000000000001</v>
@@ -3587,7 +3599,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B250">
         <v>0.127</v>
@@ -3598,7 +3610,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B251">
         <v>7.9399999999999998E-2</v>
@@ -3708,7 +3720,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B261">
         <v>0.28570000000000001</v>
@@ -3752,7 +3764,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B265">
         <v>0.38100000000000001</v>
@@ -3763,7 +3775,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B266">
         <v>0.26979999999999998</v>
@@ -3785,7 +3797,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B268">
         <v>0.46029999999999999</v>
@@ -3796,7 +3808,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>0</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="B269">
         <v>0.1905</v>
@@ -3807,7 +3819,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>0</v>
+        <v>2.1499999999999998E-2</v>
       </c>
       <c r="B270">
         <v>0.1905</v>
@@ -3818,7 +3830,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>2.0000000000000001E-4</v>
+        <v>5.1200000000000002E-2</v>
       </c>
       <c r="B271">
         <v>0.39679999999999999</v>
@@ -3829,7 +3841,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>4.0300000000000002E-2</v>
+        <v>9.0700000000000003E-2</v>
       </c>
       <c r="B272">
         <v>0.254</v>
@@ -3840,7 +3852,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>9.0999999999999998E-2</v>
+        <v>0.12</v>
       </c>
       <c r="B273">
         <v>0.26979999999999998</v>
@@ -3851,7 +3863,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>7.9000000000000001E-2</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="B274">
         <v>0.44440000000000002</v>
@@ -3862,7 +3874,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>0.13059999999999999</v>
+        <v>0.18060000000000001</v>
       </c>
       <c r="B275">
         <v>0.44440000000000002</v>
@@ -3873,7 +3885,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>0.18870000000000001</v>
+        <v>0.18090000000000001</v>
       </c>
       <c r="B276">
         <v>0.30159999999999998</v>
@@ -3884,7 +3896,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>9.9299999999999999E-2</v>
+        <v>0.1691</v>
       </c>
       <c r="B277">
         <v>0.38100000000000001</v>
@@ -3895,7 +3907,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>0.14929999999999999</v>
+        <v>0.16070000000000001</v>
       </c>
       <c r="B278">
         <v>0.36509999999999998</v>
@@ -3906,7 +3918,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>0.1295</v>
+        <v>0.16020000000000001</v>
       </c>
       <c r="B279">
         <v>0.42859999999999998</v>
@@ -3917,7 +3929,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>0.1376</v>
+        <v>0.1208</v>
       </c>
       <c r="B280">
         <v>0.36509999999999998</v>
@@ -3928,7 +3940,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>0.1145</v>
+        <v>9.8799999999999999E-2</v>
       </c>
       <c r="B281">
         <v>0.33329999999999999</v>
@@ -3939,7 +3951,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282">
-        <v>6.4500000000000002E-2</v>
+        <v>7.0300000000000001E-2</v>
       </c>
       <c r="B282">
         <v>0.3175</v>
@@ -3950,7 +3962,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>6.2E-2</v>
+        <v>5.3600000000000002E-2</v>
       </c>
       <c r="B283">
         <v>0.26979999999999998</v>
@@ -3961,7 +3973,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284">
-        <v>4.2599999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="B284">
         <v>0.34920000000000001</v>
@@ -3972,7 +3984,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>3.6799999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="B285">
         <v>0.30159999999999998</v>
@@ -3983,7 +3995,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>3.6499999999999998E-2</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="B286">
         <v>0.3175</v>
@@ -3994,7 +4006,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>6.7999999999999996E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="B287">
         <v>0.39679999999999999</v>
@@ -4005,7 +4017,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>3.0000000000000001E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="B288">
         <v>0.46029999999999999</v>
@@ -4016,7 +4028,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>2.8E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="B289">
         <v>0.44440000000000002</v>
@@ -4027,7 +4039,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>3.8999999999999998E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="B290">
         <v>0.34920000000000001</v>
@@ -4038,7 +4050,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>1.1999999999999999E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B291">
         <v>0.30159999999999998</v>
@@ -4049,7 +4061,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>1.2999999999999999E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B292">
         <v>0.38100000000000001</v>
@@ -4060,7 +4072,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>2.0000000000000001E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B293">
         <v>0.39679999999999999</v>
@@ -4071,7 +4083,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>8.9999999999999998E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B294">
         <v>0.1905</v>
@@ -4082,7 +4094,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B295">
         <v>6.3500000000000001E-2</v>
@@ -4115,7 +4127,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B298">
         <v>0.30159999999999998</v>
@@ -4148,7 +4160,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B301">
         <v>0.41270000000000001</v>
@@ -4181,7 +4193,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B304">
         <v>0.46029999999999999</v>
@@ -4192,7 +4204,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B305">
         <v>0.44440000000000002</v>
@@ -4236,7 +4248,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B309">
         <v>0.34920000000000001</v>
@@ -4247,7 +4259,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B310">
         <v>0.49209999999999998</v>
@@ -4258,7 +4270,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B311">
         <v>0.15870000000000001</v>
@@ -4291,7 +4303,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B314">
         <v>0.30159999999999998</v>
@@ -4335,7 +4347,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B318">
         <v>0.34920000000000001</v>
@@ -4357,7 +4369,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B320">
         <v>0.49209999999999998</v>
@@ -4489,7 +4501,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B332">
         <v>0.15870000000000001</v>
@@ -4511,7 +4523,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B334">
         <v>6.3500000000000001E-2</v>
@@ -4522,7 +4534,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B335">
         <v>0.1111</v>
@@ -4566,7 +4578,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B339">
         <v>0.1429</v>
@@ -4577,7 +4589,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B340">
         <v>0.33329999999999999</v>
@@ -4588,7 +4600,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B341">
         <v>0.46029999999999999</v>
@@ -4621,7 +4633,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B344">
         <v>6.3500000000000001E-2</v>
@@ -4632,7 +4644,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B345">
         <v>0.26979999999999998</v>
@@ -4654,7 +4666,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B347">
         <v>0.23810000000000001</v>
@@ -4676,7 +4688,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B349">
         <v>0.38100000000000001</v>
@@ -4687,7 +4699,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B350">
         <v>0.42859999999999998</v>
@@ -4698,7 +4710,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B351">
         <v>0</v>
@@ -4753,7 +4765,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356">
-        <v>1E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B356">
         <v>0.1905</v>
@@ -4775,7 +4787,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A358">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B358">
         <v>0.127</v>
@@ -4797,7 +4809,7 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A360">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B360">
         <v>0.36509999999999998</v>
@@ -4841,7 +4853,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="B364">
         <v>0.50790000000000002</v>
@@ -4852,7 +4864,7 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B365">
         <v>0.46029999999999999</v>
@@ -4863,7 +4875,7 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366">
-        <v>2.0000000000000001E-4</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B366">
         <v>0.49209999999999998</v>
@@ -4874,7 +4886,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B367">
         <v>0.52380000000000004</v>
@@ -4896,7 +4908,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B369">
         <v>0.254</v>
@@ -4907,7 +4919,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B370">
         <v>0.38100000000000001</v>
@@ -4951,7 +4963,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B374">
         <v>0.58730000000000004</v>
@@ -4973,7 +4985,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B376">
         <v>0.1111</v>
@@ -5006,7 +5018,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379">
-        <v>0</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B379">
         <v>0.42859999999999998</v>
@@ -5017,7 +5029,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="B380">
         <v>0.52380000000000004</v>
@@ -5028,7 +5040,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381">
-        <v>1.0200000000000001E-2</v>
+        <v>6.0699999999999997E-2</v>
       </c>
       <c r="B381">
         <v>0.23810000000000001</v>
@@ -5039,7 +5051,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382">
-        <v>2.24E-2</v>
+        <v>0.1573</v>
       </c>
       <c r="B382">
         <v>0.30159999999999998</v>
@@ -5050,7 +5062,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383">
-        <v>0.1227</v>
+        <v>0.31269999999999998</v>
       </c>
       <c r="B383">
         <v>0.28570000000000001</v>
@@ -5061,7 +5073,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384">
-        <v>0.35249999999999998</v>
+        <v>0.5887</v>
       </c>
       <c r="B384">
         <v>0.26979999999999998</v>
@@ -5072,7 +5084,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385">
-        <v>0.59830000000000005</v>
+        <v>0.7036</v>
       </c>
       <c r="B385">
         <v>0.26979999999999998</v>
@@ -5083,7 +5095,7 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386">
-        <v>1</v>
+        <v>0.7298</v>
       </c>
       <c r="B386">
         <v>0.254</v>
@@ -5094,7 +5106,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387">
-        <v>0.77459999999999996</v>
+        <v>0.63870000000000005</v>
       </c>
       <c r="B387">
         <v>0.26979999999999998</v>
@@ -5105,7 +5117,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388">
-        <v>0.70109999999999995</v>
+        <v>0.57410000000000005</v>
       </c>
       <c r="B388">
         <v>0.254</v>
@@ -5116,7 +5128,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389">
-        <v>0.70169999999999999</v>
+        <v>0.52459999999999996</v>
       </c>
       <c r="B389">
         <v>0.254</v>
@@ -5127,7 +5139,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390">
-        <v>0.53269999999999995</v>
+        <v>0.58120000000000005</v>
       </c>
       <c r="B390">
         <v>0.28570000000000001</v>
@@ -5138,7 +5150,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391">
-        <v>0.52639999999999998</v>
+        <v>0.70609999999999995</v>
       </c>
       <c r="B391">
         <v>0.30159999999999998</v>
@@ -5149,7 +5161,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392">
-        <v>0.93640000000000001</v>
+        <v>0.751</v>
       </c>
       <c r="B392">
         <v>0.254</v>
@@ -5160,7 +5172,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393">
-        <v>0.95940000000000003</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="B393">
         <v>0.22220000000000001</v>
@@ -5171,7 +5183,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394">
-        <v>0.65400000000000003</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="B394">
         <v>0.26979999999999998</v>
@@ -5182,7 +5194,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395">
-        <v>0.72199999999999998</v>
+        <v>0.47010000000000002</v>
       </c>
       <c r="B395">
         <v>0.254</v>
@@ -5193,7 +5205,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396">
-        <v>0.52949999999999997</v>
+        <v>0.32979999999999998</v>
       </c>
       <c r="B396">
         <v>0.26979999999999998</v>
@@ -5204,7 +5216,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397">
-        <v>0.44369999999999998</v>
+        <v>0.22539999999999999</v>
       </c>
       <c r="B397">
         <v>0.26979999999999998</v>
@@ -5215,7 +5227,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398">
-        <v>0.2263</v>
+        <v>0.13020000000000001</v>
       </c>
       <c r="B398">
         <v>0.28570000000000001</v>
@@ -5226,7 +5238,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399">
-        <v>0.11899999999999999</v>
+        <v>8.8400000000000006E-2</v>
       </c>
       <c r="B399">
         <v>0.26979999999999998</v>
@@ -5237,7 +5249,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400">
-        <v>0.1019</v>
+        <v>5.7799999999999997E-2</v>
       </c>
       <c r="B400">
         <v>0.23810000000000001</v>
@@ -5248,7 +5260,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401">
-        <v>8.2299999999999998E-2</v>
+        <v>3.5700000000000003E-2</v>
       </c>
       <c r="B401">
         <v>0.23810000000000001</v>
@@ -5259,7 +5271,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402">
-        <v>1.6899999999999998E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="B402">
         <v>0.22220000000000001</v>
@@ -5270,7 +5282,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403">
-        <v>2.98E-2</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="B403">
         <v>0.254</v>
@@ -5281,7 +5293,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404">
-        <v>0.01</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="B404">
         <v>0.34920000000000001</v>
@@ -5292,7 +5304,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405">
-        <v>7.7999999999999996E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="B405">
         <v>0.28570000000000001</v>
@@ -5303,7 +5315,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406">
-        <v>8.8000000000000005E-3</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="B406">
         <v>0.28570000000000001</v>
@@ -5325,7 +5337,7 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408">
-        <v>5.4000000000000003E-3</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="B408">
         <v>0.28570000000000001</v>
@@ -5336,7 +5348,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409">
-        <v>4.3E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="B409">
         <v>0.26979999999999998</v>
@@ -5347,7 +5359,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410">
-        <v>8.8999999999999999E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="B410">
         <v>0.254</v>
@@ -5358,7 +5370,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411">
-        <v>3.3E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="B411">
         <v>0.254</v>
@@ -5369,7 +5381,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412">
-        <v>2.8999999999999998E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="B412">
         <v>0.34920000000000001</v>
@@ -5380,7 +5392,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413">
-        <v>1.4E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B413">
         <v>0.28570000000000001</v>
@@ -5391,7 +5403,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414">
-        <v>2.3E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B414">
         <v>0.26979999999999998</v>
@@ -5402,7 +5414,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415">
-        <v>2.8999999999999998E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="B415">
         <v>0.23810000000000001</v>
@@ -5413,7 +5425,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416">
-        <v>1.2999999999999999E-3</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="B416">
         <v>0.30159999999999998</v>
@@ -5435,7 +5447,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418">
-        <v>2.9999999999999997E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B418">
         <v>0.33329999999999999</v>
@@ -5446,7 +5458,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419">
-        <v>8.9999999999999998E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B419">
         <v>0.28570000000000001</v>
@@ -5457,7 +5469,7 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420">
-        <v>5.0000000000000001E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B420">
         <v>0.26979999999999998</v>
@@ -5468,7 +5480,7 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B421">
         <v>0.254</v>
@@ -5512,7 +5524,7 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A425">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B425">
         <v>0.22220000000000001</v>
@@ -5523,7 +5535,7 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A426">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B426">
         <v>0.28570000000000001</v>
@@ -5578,7 +5590,7 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A431">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B431">
         <v>0.34920000000000001</v>
@@ -5600,7 +5612,7 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A433">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B433">
         <v>0.6825</v>
@@ -5611,7 +5623,7 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A434">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B434">
         <v>0.53969999999999996</v>
@@ -5644,7 +5656,7 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A437">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B437">
         <v>6.3500000000000001E-2</v>
@@ -5677,7 +5689,7 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A440">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B440">
         <v>0.34920000000000001</v>
@@ -5688,7 +5700,7 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A441">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B441">
         <v>0.63490000000000002</v>
@@ -5721,7 +5733,7 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A444">
-        <v>2.9999999999999997E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B444">
         <v>0.1429</v>
@@ -5732,7 +5744,7 @@
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A445">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B445">
         <v>0.17460000000000001</v>
@@ -5743,7 +5755,7 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A446">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B446">
         <v>0.1429</v>
@@ -5776,7 +5788,7 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A449">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B449">
         <v>0.53969999999999996</v>
@@ -5831,7 +5843,7 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A454">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B454">
         <v>0.34920000000000001</v>
@@ -5842,7 +5854,7 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A455">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B455">
         <v>0.58730000000000004</v>
@@ -5864,7 +5876,7 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A457">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B457">
         <v>0.28570000000000001</v>
@@ -5908,7 +5920,7 @@
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A461">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B461">
         <v>0.33329999999999999</v>
@@ -5941,7 +5953,7 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A464">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B464">
         <v>0.36509999999999998</v>
@@ -5963,7 +5975,7 @@
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A466">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B466">
         <v>0.22220000000000001</v>
@@ -6007,7 +6019,7 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A470">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B470">
         <v>0.50790000000000002</v>
@@ -6018,7 +6030,7 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A471">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B471">
         <v>0.63490000000000002</v>
@@ -6040,7 +6052,7 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A473">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B473">
         <v>0.1905</v>
@@ -6106,7 +6118,7 @@
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B479">
         <v>0.71430000000000005</v>
@@ -6128,7 +6140,7 @@
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B481">
         <v>9.5200000000000007E-2</v>
@@ -6139,7 +6151,7 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A482">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B482">
         <v>0.44440000000000002</v>
@@ -6150,7 +6162,7 @@
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A483">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B483">
         <v>0.254</v>
@@ -6161,7 +6173,7 @@
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A484">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B484">
         <v>0.63490000000000002</v>
@@ -6172,7 +6184,7 @@
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>1E-4</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="B485">
         <v>0.60319999999999996</v>
@@ -6183,7 +6195,7 @@
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A486">
-        <v>1E-4</v>
+        <v>2.46E-2</v>
       </c>
       <c r="B486">
         <v>0.50790000000000002</v>
@@ -6194,7 +6206,7 @@
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>1.37E-2</v>
+        <v>0.1331</v>
       </c>
       <c r="B487">
         <v>0.36509999999999998</v>
@@ -6205,7 +6217,7 @@
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A488">
-        <v>0.1017</v>
+        <v>0.28820000000000001</v>
       </c>
       <c r="B488">
         <v>0.20630000000000001</v>
@@ -6216,7 +6228,7 @@
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>0.52029999999999998</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="B489">
         <v>0.1905</v>
@@ -6227,7 +6239,7 @@
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A490">
-        <v>0.63290000000000002</v>
+        <v>0.40050000000000002</v>
       </c>
       <c r="B490">
         <v>0.20630000000000001</v>
@@ -6238,7 +6250,7 @@
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>0.56179999999999997</v>
+        <v>0.34939999999999999</v>
       </c>
       <c r="B491">
         <v>0.20630000000000001</v>
@@ -6249,7 +6261,7 @@
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A492">
-        <v>0.61070000000000002</v>
+        <v>0.41570000000000001</v>
       </c>
       <c r="B492">
         <v>0.1905</v>
@@ -6260,7 +6272,7 @@
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>0.58660000000000001</v>
+        <v>0.36220000000000002</v>
       </c>
       <c r="B493">
         <v>0.15870000000000001</v>
@@ -6271,7 +6283,7 @@
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A494">
-        <v>0.64559999999999995</v>
+        <v>0.40360000000000001</v>
       </c>
       <c r="B494">
         <v>0.1429</v>
@@ -6282,7 +6294,7 @@
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>0.48139999999999999</v>
+        <v>0.32040000000000002</v>
       </c>
       <c r="B495">
         <v>0.15870000000000001</v>
@@ -6293,7 +6305,7 @@
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A496">
-        <v>0.59819999999999995</v>
+        <v>0.3019</v>
       </c>
       <c r="B496">
         <v>0.1429</v>
@@ -6304,7 +6316,7 @@
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A497">
-        <v>0.31009999999999999</v>
+        <v>0.22259999999999999</v>
       </c>
       <c r="B497">
         <v>0.1429</v>
@@ -6315,7 +6327,7 @@
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A498">
-        <v>0.3468</v>
+        <v>0.2046</v>
       </c>
       <c r="B498">
         <v>0.1429</v>
@@ -6326,7 +6338,7 @@
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>0.2928</v>
+        <v>0.1933</v>
       </c>
       <c r="B499">
         <v>0.1429</v>
@@ -6337,7 +6349,7 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A500">
-        <v>0.27029999999999998</v>
+        <v>0.15429999999999999</v>
       </c>
       <c r="B500">
         <v>0.15870000000000001</v>
@@ -6348,7 +6360,7 @@
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>0.26140000000000002</v>
+        <v>0.11840000000000001</v>
       </c>
       <c r="B501">
         <v>0.20630000000000001</v>
@@ -6359,7 +6371,7 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>0.13070000000000001</v>
+        <v>6.3299999999999995E-2</v>
       </c>
       <c r="B502">
         <v>0.22220000000000001</v>
@@ -6370,7 +6382,7 @@
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>0.1055</v>
+        <v>3.56E-2</v>
       </c>
       <c r="B503">
         <v>0.1429</v>
@@ -6381,7 +6393,7 @@
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>3.8399999999999997E-2</v>
+        <v>1.54E-2</v>
       </c>
       <c r="B504">
         <v>0.15870000000000001</v>
@@ -6392,7 +6404,7 @@
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A505">
-        <v>1.3899999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="B505">
         <v>0.20630000000000001</v>
@@ -6403,7 +6415,7 @@
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>1.35E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="B506">
         <v>0.1905</v>
@@ -6414,7 +6426,7 @@
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A507">
-        <v>7.1000000000000004E-3</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="B507">
         <v>0.20630000000000001</v>
@@ -6425,7 +6437,7 @@
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>4.8999999999999998E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="B508">
         <v>0.15870000000000001</v>
@@ -6436,7 +6448,7 @@
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>2.3999999999999998E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B509">
         <v>0.22220000000000001</v>
@@ -6458,7 +6470,7 @@
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>5.9999999999999995E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B511">
         <v>0.22220000000000001</v>
@@ -6469,7 +6481,7 @@
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A512">
-        <v>1.1999999999999999E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="B512">
         <v>0.23810000000000001</v>
@@ -6480,7 +6492,7 @@
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A513">
-        <v>4.0000000000000002E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B513">
         <v>0.36509999999999998</v>
@@ -6491,7 +6503,7 @@
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A514">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B514">
         <v>0.39679999999999999</v>
@@ -6502,7 +6514,7 @@
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A515">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B515">
         <v>0.44440000000000002</v>
@@ -6513,7 +6525,7 @@
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A516">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B516">
         <v>0.3175</v>
@@ -6524,7 +6536,7 @@
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A517">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B517">
         <v>0.33329999999999999</v>
@@ -6546,7 +6558,7 @@
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A519">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B519">
         <v>0.41270000000000001</v>
@@ -6557,7 +6569,7 @@
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A520">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B520">
         <v>0.36509999999999998</v>
@@ -6601,7 +6613,7 @@
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A524">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="B524">
         <v>0.22220000000000001</v>
@@ -6645,7 +6657,7 @@
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A528">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B528">
         <v>0.47620000000000001</v>
@@ -6656,7 +6668,7 @@
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A529">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B529">
         <v>0.47620000000000001</v>
@@ -6667,7 +6679,7 @@
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A530">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B530">
         <v>0.46029999999999999</v>
@@ -6678,7 +6690,7 @@
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A531">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B531">
         <v>0.57140000000000002</v>
@@ -6700,7 +6712,7 @@
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A533">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B533">
         <v>0.33329999999999999</v>
@@ -6733,7 +6745,7 @@
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A536">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B536">
         <v>0.746</v>
@@ -6766,7 +6778,7 @@
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A539">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B539">
         <v>0.36509999999999998</v>
@@ -6777,7 +6789,7 @@
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A540">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B540">
         <v>0.39679999999999999</v>
@@ -6788,7 +6800,7 @@
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A541">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B541">
         <v>0.47620000000000001</v>
@@ -6799,7 +6811,7 @@
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A542">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B542">
         <v>0.58730000000000004</v>
@@ -6810,7 +6822,7 @@
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A543">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B543">
         <v>0.90480000000000005</v>
@@ -6821,7 +6833,7 @@
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A544">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B544">
         <v>0.52380000000000004</v>
@@ -6876,7 +6888,7 @@
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A549">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B549">
         <v>0.69840000000000002</v>
@@ -6953,7 +6965,7 @@
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A556">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="B556">
         <v>0.60319999999999996</v>

</xml_diff>

<commit_message>
update HPS and Propose
</commit_message>
<xml_diff>
--- a/TK/thongKe.xlsx
+++ b/TK/thongKe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Class\ky2_2122\XL tín hiệu số\CK\TK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Class\ky1_2122\XL tín hiệu số\CK\TK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B94BF0-5339-4F18-A4F2-78525AC8E6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47248193-F14A-4265-9FD0-88EF90D5AAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="622" xr2:uid="{8A0C4B13-D321-42AC-9D1D-8AEB5029EB76}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="622" activeTab="3" xr2:uid="{8A0C4B13-D321-42AC-9D1D-8AEB5029EB76}"/>
   </bookViews>
   <sheets>
     <sheet name="30FTN" sheetId="1" r:id="rId1"/>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F6D3C5-97A1-4A55-9E07-2325A699C218}">
   <dimension ref="A1:M677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1001,8 +1001,8 @@
         <v>9</v>
       </c>
       <c r="G18">
-        <f xml:space="preserve"> ((F15 + 3 * H15) + (F16 - 3 * H16)) / 2</f>
-        <v>7.1723192010183984E-2</v>
+        <f xml:space="preserve"> ((F15 + H15) + (F16 - 4 * H16)) / 2</f>
+        <v>5.0412729958818459E-2</v>
       </c>
       <c r="L18">
         <f xml:space="preserve"> ((K15 + M15) + (K16 - M16)) / 2</f>
@@ -7967,8 +7967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F811CF6-3847-43D8-916F-CCE6BE5BB2F7}">
   <dimension ref="A1:M580"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8534,8 +8534,8 @@
         <v>9</v>
       </c>
       <c r="G18">
-        <f xml:space="preserve"> ((F15 + 3 * H15) + (F16 - 3 * H16)) / 2</f>
-        <v>1.6645559872139757E-2</v>
+        <f xml:space="preserve"> ((F15 + H15) + (F16 - 4 * H16)) / 2</f>
+        <v>-9.0093969825561261E-3</v>
       </c>
       <c r="L18">
         <f xml:space="preserve"> ((K15 + M15) + (K16 - M16)) / 2</f>
@@ -14715,7 +14715,7 @@
   <dimension ref="A1:M926"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -15284,8 +15284,8 @@
         <v>9</v>
       </c>
       <c r="G18">
-        <f xml:space="preserve"> ((F15 + 3 * H15) + (F16 - 3 * H16)) / 2</f>
-        <v>6.1794580307039819E-2</v>
+        <f xml:space="preserve"> ((F15 + H15) + (F16 - 4 * H16)) / 2</f>
+        <v>3.9007014149959836E-2</v>
       </c>
       <c r="L18">
         <f xml:space="preserve"> ((K15 + M15) + (K16 - M16)) / 2</f>
@@ -24242,8 +24242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030D9D64-E9AE-4B24-81A1-9A111E125227}">
   <dimension ref="A1:M742"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -24809,8 +24809,8 @@
         <v>9</v>
       </c>
       <c r="G18">
-        <f xml:space="preserve"> ((F15 + 3 * H15) + (F16 - 3 * H16)) / 2</f>
-        <v>1.3222873050385862E-2</v>
+        <f xml:space="preserve"> ((F15 + H15) + (F16 - 4 * H16)) / 2</f>
+        <v>-1.5166351502991293E-2</v>
       </c>
       <c r="L18">
         <f xml:space="preserve"> ((K15 + M15) + (K16 - M16)) / 2</f>

</xml_diff>